<commit_message>
revamp macrobuilder use of template, get dossier class working
</commit_message>
<xml_diff>
--- a/startup/xlsx/doublewheel.xlsx
+++ b/startup/xlsx/doublewheel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="set1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="set2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="set3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="dw1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="dw2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="dw3" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Version history" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -989,9 +989,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>96480</xdr:colOff>
+      <xdr:colOff>96120</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1000,8 +1000,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3350160" y="10725120"/>
-          <a:ext cx="6643800" cy="2261520"/>
+          <a:off x="3350520" y="10725120"/>
+          <a:ext cx="6644520" cy="2261160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1248,9 +1248,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1100160</xdr:colOff>
+      <xdr:colOff>1099800</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1263,8 +1263,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1292760" y="10772280"/>
-          <a:ext cx="1836000" cy="2448360"/>
+          <a:off x="1293480" y="10772280"/>
+          <a:ext cx="1835640" cy="2448000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1290,9 +1290,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>96480</xdr:colOff>
+      <xdr:colOff>96120</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1301,688 +1301,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3350160" y="10725120"/>
-          <a:ext cx="6643800" cy="2261520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="73080">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>Instructio</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>ns:</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>1. Add the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>names of all </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>team </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>members to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>the green </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>box in row 1</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>2. Default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>values for all </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>parameters </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>go in line 6</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>3. Sample-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>specific </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>parameters </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>are entered </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>4. Default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>values from </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>line 6 will be </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>used for all </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>cells left </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>blank in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>5. Specify </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>motor/slit </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>positions in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>columns </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>R,S,T; leave </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>blank for no </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>motion</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Specify </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>detector </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>position in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>column U, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>blank means </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>not move</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>the detector </a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Do not </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>add rows </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>above row 7</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>7. Do not </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>add columns </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>before </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>column AE</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>8. The wheel </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>is correctly </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>mounted if </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>the numbers </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>can be read </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>when facing </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>the wheel</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>676440</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1100160</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1292760" y="10772280"/>
-          <a:ext cx="1836000" cy="2448360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>96480</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3350160" y="10725120"/>
-          <a:ext cx="6643800" cy="2261520"/>
+          <a:off x="3350520" y="10725120"/>
+          <a:ext cx="6644520" cy="2261160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2229,9 +1549,310 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1100160</xdr:colOff>
+      <xdr:colOff>1099800</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1293480" y="10772280"/>
+          <a:ext cx="1835640" cy="2448000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66600</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>96120</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>118080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3350520" y="10725120"/>
+          <a:ext cx="6644520" cy="2261160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="73080">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFillTx/>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>Instructions:</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>2. Default values for all parameters go in line 6</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Specify detector position in column U, blank means to </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>not move</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t> the detector </a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Do not add rows above row 7</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>7. Do not add columns before column AE</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>8. The wheel is correctly mounted if the numbers can be read when facing the wheel</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676440</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1099800</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2244,8 +1865,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1292760" y="10772280"/>
-          <a:ext cx="1836000" cy="2448360"/>
+          <a:off x="1293480" y="10772280"/>
+          <a:ext cx="1835640" cy="2448000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2267,7 +1888,7 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -2275,7 +1896,7 @@
       <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -4303,7 +3924,7 @@
       <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -6306,7 +5927,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6323,7 +5944,7 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -6331,7 +5952,7 @@
       <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -8334,7 +7955,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -8355,7 +7976,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>

</xml_diff>

<commit_message>
touching up some things...
</commit_message>
<xml_diff>
--- a/startup/xlsx/doublewheel.xlsx
+++ b/startup/xlsx/doublewheel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="dw1" sheetId="1" state="visible" r:id="rId2"/>
@@ -984,14 +984,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>96120</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:colOff>95400</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1000,8 +1000,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3350520" y="10725120"/>
-          <a:ext cx="6644520" cy="2261160"/>
+          <a:off x="3352680" y="10725120"/>
+          <a:ext cx="6645240" cy="2260440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1243,14 +1243,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>676440</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1099800</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:colOff>1099080</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1263,8 +1263,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1293480" y="10772280"/>
-          <a:ext cx="1835640" cy="2448000"/>
+          <a:off x="1295280" y="10772280"/>
+          <a:ext cx="1834920" cy="2447280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1285,14 +1285,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>96120</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:colOff>95400</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1301,8 +1301,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3350520" y="10725120"/>
-          <a:ext cx="6644520" cy="2261160"/>
+          <a:off x="3352680" y="10725120"/>
+          <a:ext cx="6645240" cy="2260440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1544,14 +1544,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>676440</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1099800</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:colOff>1099080</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1564,8 +1564,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1293480" y="10772280"/>
-          <a:ext cx="1835640" cy="2448000"/>
+          <a:off x="1295280" y="10772280"/>
+          <a:ext cx="1834920" cy="2447280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1586,14 +1586,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>96120</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:colOff>95400</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1602,8 +1602,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3350520" y="10725120"/>
-          <a:ext cx="6644520" cy="2261160"/>
+          <a:off x="3352680" y="10725120"/>
+          <a:ext cx="6645240" cy="2260440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1845,14 +1845,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>676440</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1099800</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:colOff>1099080</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1865,8 +1865,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1293480" y="10772280"/>
-          <a:ext cx="1835640" cy="2448000"/>
+          <a:off x="1295280" y="10772280"/>
+          <a:ext cx="1834920" cy="2447280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1888,15 +1888,15 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="U6" activeCellId="0" sqref="R6:U54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -3019,7 +3019,7 @@
       <c r="AA30" s="58"/>
       <c r="AB30" s="59"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="47" t="n">
         <v>1</v>
       </c>
@@ -3052,7 +3052,7 @@
       <c r="AA31" s="58"/>
       <c r="AB31" s="59"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="47" t="n">
         <v>2</v>
       </c>
@@ -3085,7 +3085,7 @@
       <c r="AA32" s="58"/>
       <c r="AB32" s="59"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="47" t="n">
         <v>3</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="AA33" s="58"/>
       <c r="AB33" s="59"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="47" t="n">
         <v>4</v>
       </c>
@@ -3151,7 +3151,7 @@
       <c r="AA34" s="58"/>
       <c r="AB34" s="59"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="47" t="n">
         <v>5</v>
       </c>
@@ -3184,7 +3184,7 @@
       <c r="AA35" s="58"/>
       <c r="AB35" s="59"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="47" t="n">
         <v>6</v>
       </c>
@@ -3217,7 +3217,7 @@
       <c r="AA36" s="58"/>
       <c r="AB36" s="59"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="47" t="n">
         <v>7</v>
       </c>
@@ -3250,7 +3250,7 @@
       <c r="AA37" s="58"/>
       <c r="AB37" s="59"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="47" t="n">
         <v>8</v>
       </c>
@@ -3283,7 +3283,7 @@
       <c r="AA38" s="58"/>
       <c r="AB38" s="59"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="47" t="n">
         <v>9</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="AA39" s="58"/>
       <c r="AB39" s="59"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="47" t="n">
         <v>10</v>
       </c>
@@ -3349,7 +3349,7 @@
       <c r="AA40" s="58"/>
       <c r="AB40" s="59"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="47" t="n">
         <v>11</v>
       </c>
@@ -3382,7 +3382,7 @@
       <c r="AA41" s="58"/>
       <c r="AB41" s="59"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="47" t="n">
         <v>12</v>
       </c>
@@ -3415,7 +3415,7 @@
       <c r="AA42" s="58"/>
       <c r="AB42" s="59"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="47" t="n">
         <v>13</v>
       </c>
@@ -3448,7 +3448,7 @@
       <c r="AA43" s="58"/>
       <c r="AB43" s="59"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="47" t="n">
         <v>14</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="AA44" s="58"/>
       <c r="AB44" s="59"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="47" t="n">
         <v>15</v>
       </c>
@@ -3514,7 +3514,7 @@
       <c r="AA45" s="58"/>
       <c r="AB45" s="59"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="47" t="n">
         <v>16</v>
       </c>
@@ -3547,7 +3547,7 @@
       <c r="AA46" s="58"/>
       <c r="AB46" s="59"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="47" t="n">
         <v>17</v>
       </c>
@@ -3580,7 +3580,7 @@
       <c r="AA47" s="58"/>
       <c r="AB47" s="59"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="47" t="n">
         <v>18</v>
       </c>
@@ -3613,7 +3613,7 @@
       <c r="AA48" s="58"/>
       <c r="AB48" s="59"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="47" t="n">
         <v>19</v>
       </c>
@@ -3646,7 +3646,7 @@
       <c r="AA49" s="58"/>
       <c r="AB49" s="59"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="47" t="n">
         <v>20</v>
       </c>
@@ -3679,7 +3679,7 @@
       <c r="AA50" s="58"/>
       <c r="AB50" s="59"/>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="47" t="n">
         <v>21</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="AA51" s="58"/>
       <c r="AB51" s="59"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="47" t="n">
         <v>22</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="AA52" s="58"/>
       <c r="AB52" s="59"/>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="47" t="n">
         <v>23</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="AA53" s="58"/>
       <c r="AB53" s="59"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="47" t="n">
         <v>24</v>
       </c>
@@ -3827,7 +3827,7 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="17">
+  <dataValidations count="15">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -3852,17 +3852,9 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6" type="decimal">
-      <formula1>10</formula1>
-      <formula2>400</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="decimal">
-      <formula1>-150</formula1>
-      <formula2>150</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
@@ -3876,10 +3868,6 @@
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6" type="decimal">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
@@ -3892,9 +3880,13 @@
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:U72" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3921,10 +3913,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="U6" activeCellId="0" sqref="R6:U54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -5047,7 +5039,7 @@
       <c r="AA30" s="58"/>
       <c r="AB30" s="59"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="47" t="n">
         <v>1</v>
       </c>
@@ -5080,7 +5072,7 @@
       <c r="AA31" s="58"/>
       <c r="AB31" s="59"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="47" t="n">
         <v>2</v>
       </c>
@@ -5113,7 +5105,7 @@
       <c r="AA32" s="58"/>
       <c r="AB32" s="59"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="47" t="n">
         <v>3</v>
       </c>
@@ -5146,7 +5138,7 @@
       <c r="AA33" s="58"/>
       <c r="AB33" s="59"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="47" t="n">
         <v>4</v>
       </c>
@@ -5179,7 +5171,7 @@
       <c r="AA34" s="58"/>
       <c r="AB34" s="59"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="47" t="n">
         <v>5</v>
       </c>
@@ -5212,7 +5204,7 @@
       <c r="AA35" s="58"/>
       <c r="AB35" s="59"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="47" t="n">
         <v>6</v>
       </c>
@@ -5245,7 +5237,7 @@
       <c r="AA36" s="58"/>
       <c r="AB36" s="59"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="47" t="n">
         <v>7</v>
       </c>
@@ -5278,7 +5270,7 @@
       <c r="AA37" s="58"/>
       <c r="AB37" s="59"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="47" t="n">
         <v>8</v>
       </c>
@@ -5311,7 +5303,7 @@
       <c r="AA38" s="58"/>
       <c r="AB38" s="59"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="47" t="n">
         <v>9</v>
       </c>
@@ -5344,7 +5336,7 @@
       <c r="AA39" s="58"/>
       <c r="AB39" s="59"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="47" t="n">
         <v>10</v>
       </c>
@@ -5377,7 +5369,7 @@
       <c r="AA40" s="58"/>
       <c r="AB40" s="59"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="47" t="n">
         <v>11</v>
       </c>
@@ -5410,7 +5402,7 @@
       <c r="AA41" s="58"/>
       <c r="AB41" s="59"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="47" t="n">
         <v>12</v>
       </c>
@@ -5443,7 +5435,7 @@
       <c r="AA42" s="58"/>
       <c r="AB42" s="59"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="47" t="n">
         <v>13</v>
       </c>
@@ -5476,7 +5468,7 @@
       <c r="AA43" s="58"/>
       <c r="AB43" s="59"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="47" t="n">
         <v>14</v>
       </c>
@@ -5509,7 +5501,7 @@
       <c r="AA44" s="58"/>
       <c r="AB44" s="59"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="47" t="n">
         <v>15</v>
       </c>
@@ -5542,7 +5534,7 @@
       <c r="AA45" s="58"/>
       <c r="AB45" s="59"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="47" t="n">
         <v>16</v>
       </c>
@@ -5575,7 +5567,7 @@
       <c r="AA46" s="58"/>
       <c r="AB46" s="59"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="47" t="n">
         <v>17</v>
       </c>
@@ -5608,7 +5600,7 @@
       <c r="AA47" s="58"/>
       <c r="AB47" s="59"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="47" t="n">
         <v>18</v>
       </c>
@@ -5641,7 +5633,7 @@
       <c r="AA48" s="58"/>
       <c r="AB48" s="59"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="47" t="n">
         <v>19</v>
       </c>
@@ -5674,7 +5666,7 @@
       <c r="AA49" s="58"/>
       <c r="AB49" s="59"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="47" t="n">
         <v>20</v>
       </c>
@@ -5707,7 +5699,7 @@
       <c r="AA50" s="58"/>
       <c r="AB50" s="59"/>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="47" t="n">
         <v>21</v>
       </c>
@@ -5740,7 +5732,7 @@
       <c r="AA51" s="58"/>
       <c r="AB51" s="59"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="47" t="n">
         <v>22</v>
       </c>
@@ -5773,7 +5765,7 @@
       <c r="AA52" s="58"/>
       <c r="AB52" s="59"/>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="47" t="n">
         <v>23</v>
       </c>
@@ -5806,7 +5798,7 @@
       <c r="AA53" s="58"/>
       <c r="AB53" s="59"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="47" t="n">
         <v>24</v>
       </c>
@@ -5855,7 +5847,7 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="17">
+  <dataValidations count="15">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -5880,17 +5872,9 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6" type="decimal">
-      <formula1>10</formula1>
-      <formula2>400</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="decimal">
-      <formula1>-150</formula1>
-      <formula2>150</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
@@ -5904,10 +5888,6 @@
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6" type="decimal">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
@@ -5920,9 +5900,13 @@
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:U72" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5944,15 +5928,15 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="O43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="U6" activeCellId="0" sqref="R6:U54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -7075,7 +7059,7 @@
       <c r="AA30" s="58"/>
       <c r="AB30" s="59"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="47" t="n">
         <v>1</v>
       </c>
@@ -7108,7 +7092,7 @@
       <c r="AA31" s="58"/>
       <c r="AB31" s="59"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="47" t="n">
         <v>2</v>
       </c>
@@ -7141,7 +7125,7 @@
       <c r="AA32" s="58"/>
       <c r="AB32" s="59"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="47" t="n">
         <v>3</v>
       </c>
@@ -7174,7 +7158,7 @@
       <c r="AA33" s="58"/>
       <c r="AB33" s="59"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="47" t="n">
         <v>4</v>
       </c>
@@ -7207,7 +7191,7 @@
       <c r="AA34" s="58"/>
       <c r="AB34" s="59"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="47" t="n">
         <v>5</v>
       </c>
@@ -7240,7 +7224,7 @@
       <c r="AA35" s="58"/>
       <c r="AB35" s="59"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="47" t="n">
         <v>6</v>
       </c>
@@ -7273,7 +7257,7 @@
       <c r="AA36" s="58"/>
       <c r="AB36" s="59"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="47" t="n">
         <v>7</v>
       </c>
@@ -7306,7 +7290,7 @@
       <c r="AA37" s="58"/>
       <c r="AB37" s="59"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="47" t="n">
         <v>8</v>
       </c>
@@ -7339,7 +7323,7 @@
       <c r="AA38" s="58"/>
       <c r="AB38" s="59"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="47" t="n">
         <v>9</v>
       </c>
@@ -7372,7 +7356,7 @@
       <c r="AA39" s="58"/>
       <c r="AB39" s="59"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="47" t="n">
         <v>10</v>
       </c>
@@ -7405,7 +7389,7 @@
       <c r="AA40" s="58"/>
       <c r="AB40" s="59"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="47" t="n">
         <v>11</v>
       </c>
@@ -7438,7 +7422,7 @@
       <c r="AA41" s="58"/>
       <c r="AB41" s="59"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="47" t="n">
         <v>12</v>
       </c>
@@ -7471,7 +7455,7 @@
       <c r="AA42" s="58"/>
       <c r="AB42" s="59"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="47" t="n">
         <v>13</v>
       </c>
@@ -7504,7 +7488,7 @@
       <c r="AA43" s="58"/>
       <c r="AB43" s="59"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="47" t="n">
         <v>14</v>
       </c>
@@ -7537,7 +7521,7 @@
       <c r="AA44" s="58"/>
       <c r="AB44" s="59"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="47" t="n">
         <v>15</v>
       </c>
@@ -7570,7 +7554,7 @@
       <c r="AA45" s="58"/>
       <c r="AB45" s="59"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="47" t="n">
         <v>16</v>
       </c>
@@ -7603,7 +7587,7 @@
       <c r="AA46" s="58"/>
       <c r="AB46" s="59"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="47" t="n">
         <v>17</v>
       </c>
@@ -7636,7 +7620,7 @@
       <c r="AA47" s="58"/>
       <c r="AB47" s="59"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="47" t="n">
         <v>18</v>
       </c>
@@ -7669,7 +7653,7 @@
       <c r="AA48" s="58"/>
       <c r="AB48" s="59"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="47" t="n">
         <v>19</v>
       </c>
@@ -7702,7 +7686,7 @@
       <c r="AA49" s="58"/>
       <c r="AB49" s="59"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="47" t="n">
         <v>20</v>
       </c>
@@ -7735,7 +7719,7 @@
       <c r="AA50" s="58"/>
       <c r="AB50" s="59"/>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="47" t="n">
         <v>21</v>
       </c>
@@ -7768,7 +7752,7 @@
       <c r="AA51" s="58"/>
       <c r="AB51" s="59"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="47" t="n">
         <v>22</v>
       </c>
@@ -7801,7 +7785,7 @@
       <c r="AA52" s="58"/>
       <c r="AB52" s="59"/>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="47" t="n">
         <v>23</v>
       </c>
@@ -7834,7 +7818,7 @@
       <c r="AA53" s="58"/>
       <c r="AB53" s="59"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="47" t="n">
         <v>24</v>
       </c>
@@ -7883,7 +7867,7 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="17">
+  <dataValidations count="15">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -7908,18 +7892,6 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
-      <formula1>-0.1</formula1>
-      <formula2>8</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6" type="decimal">
-      <formula1>10</formula1>
-      <formula2>400</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="decimal">
-      <formula1>-150</formula1>
-      <formula2>150</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
@@ -7931,10 +7903,6 @@
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6" type="decimal">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
@@ -7948,9 +7916,17 @@
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:U72" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7973,10 +7949,10 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="R6:U54 A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>

</xml_diff>

<commit_message>
parameter to loop over entire spreadsheet
</commit_message>
<xml_diff>
--- a/startup/xlsx/doublewheel.xlsx
+++ b/startup/xlsx/doublewheel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dw1" sheetId="1" state="visible" r:id="rId2"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="71">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add element to filename?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of repetitions</t>
   </si>
   <si>
     <t xml:space="preserve">File name</t>
@@ -188,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">Filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of repetitions</t>
   </si>
   <si>
     <t xml:space="preserve">Starting scan number</t>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">Added LakeShore 331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loop over entire macro</t>
   </si>
 </sst>
 </file>
@@ -706,12 +709,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -997,9 +1000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>94320</xdr:colOff>
+      <xdr:colOff>93960</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1008,8 +1011,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3355200" y="10725120"/>
-          <a:ext cx="6646680" cy="2259360"/>
+          <a:off x="3356280" y="10725120"/>
+          <a:ext cx="6648120" cy="2259000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1256,9 +1259,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098360</xdr:colOff>
+      <xdr:colOff>1098000</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:rowOff>50400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1271,8 +1274,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1298160" y="10772280"/>
-          <a:ext cx="1833840" cy="2446200"/>
+          <a:off x="1299600" y="10772280"/>
+          <a:ext cx="1833480" cy="2445840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1298,9 +1301,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>94320</xdr:colOff>
+      <xdr:colOff>93960</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1309,8 +1312,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3355200" y="10725120"/>
-          <a:ext cx="6646680" cy="2259360"/>
+          <a:off x="3356280" y="10725120"/>
+          <a:ext cx="6648120" cy="2259000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1557,9 +1560,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098360</xdr:colOff>
+      <xdr:colOff>1098000</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:rowOff>50400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1572,8 +1575,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1298160" y="10772280"/>
-          <a:ext cx="1833840" cy="2446200"/>
+          <a:off x="1299600" y="10772280"/>
+          <a:ext cx="1833480" cy="2445840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1599,9 +1602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>94320</xdr:colOff>
+      <xdr:colOff>93960</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1610,8 +1613,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3355200" y="10725120"/>
-          <a:ext cx="6646680" cy="2259360"/>
+          <a:off x="3356280" y="10725120"/>
+          <a:ext cx="6648120" cy="2259000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1858,9 +1861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098360</xdr:colOff>
+      <xdr:colOff>1098000</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:rowOff>50400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1873,8 +1876,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1298160" y="10772280"/>
-          <a:ext cx="1833840" cy="2446200"/>
+          <a:off x="1299600" y="10772280"/>
+          <a:ext cx="1833480" cy="2445840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1897,14 +1900,14 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="P43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="AE1" activeCellId="0" sqref="AE1"/>
+      <selection pane="bottomRight" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -1959,7 +1962,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 8</v>
+        <v>Version: 9</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -1983,77 +1986,81 @@
       <c r="M2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="11"/>
+      <c r="N2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="10"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
-      <c r="AA2" s="11"/>
+      <c r="AA2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="10"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
-      <c r="AA3" s="11"/>
+      <c r="AA3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
       <c r="R4" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
       <c r="U4" s="16"/>
       <c r="V4" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W4" s="16"/>
       <c r="X4" s="16"/>
@@ -2061,26 +2068,26 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
       <c r="AB4" s="17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AC4" s="17"/>
       <c r="AD4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>20</v>
@@ -2224,7 +2231,8 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="45" t="b">
+      <c r="Z6" s="45" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AA6" s="46" t="n">
@@ -2258,7 +2266,7 @@
       <c r="O7" s="54"/>
       <c r="P7" s="29"/>
       <c r="Q7" s="55"/>
-      <c r="T7" s="10"/>
+      <c r="T7" s="11"/>
       <c r="U7" s="56"/>
       <c r="V7" s="57"/>
       <c r="W7" s="58"/>
@@ -2291,7 +2299,7 @@
       <c r="O8" s="54"/>
       <c r="P8" s="29"/>
       <c r="Q8" s="55"/>
-      <c r="T8" s="10"/>
+      <c r="T8" s="11"/>
       <c r="U8" s="56"/>
       <c r="V8" s="57"/>
       <c r="W8" s="58"/>
@@ -2324,7 +2332,7 @@
       <c r="O9" s="54"/>
       <c r="P9" s="29"/>
       <c r="Q9" s="55"/>
-      <c r="T9" s="10"/>
+      <c r="T9" s="11"/>
       <c r="U9" s="56"/>
       <c r="V9" s="57"/>
       <c r="W9" s="58"/>
@@ -2357,7 +2365,7 @@
       <c r="O10" s="54"/>
       <c r="P10" s="29"/>
       <c r="Q10" s="55"/>
-      <c r="T10" s="10"/>
+      <c r="T10" s="11"/>
       <c r="U10" s="56"/>
       <c r="V10" s="57"/>
       <c r="W10" s="58"/>
@@ -2390,7 +2398,7 @@
       <c r="O11" s="54"/>
       <c r="P11" s="29"/>
       <c r="Q11" s="55"/>
-      <c r="T11" s="10"/>
+      <c r="T11" s="11"/>
       <c r="U11" s="56"/>
       <c r="V11" s="57"/>
       <c r="W11" s="58"/>
@@ -2423,7 +2431,7 @@
       <c r="O12" s="54"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="55"/>
-      <c r="T12" s="10"/>
+      <c r="T12" s="11"/>
       <c r="U12" s="56"/>
       <c r="V12" s="57"/>
       <c r="W12" s="58"/>
@@ -2456,7 +2464,7 @@
       <c r="O13" s="54"/>
       <c r="P13" s="29"/>
       <c r="Q13" s="55"/>
-      <c r="T13" s="10"/>
+      <c r="T13" s="11"/>
       <c r="U13" s="56"/>
       <c r="V13" s="57"/>
       <c r="W13" s="58"/>
@@ -2489,7 +2497,7 @@
       <c r="O14" s="54"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="55"/>
-      <c r="T14" s="10"/>
+      <c r="T14" s="11"/>
       <c r="U14" s="56"/>
       <c r="V14" s="57"/>
       <c r="W14" s="58"/>
@@ -2522,7 +2530,7 @@
       <c r="O15" s="54"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="55"/>
-      <c r="T15" s="10"/>
+      <c r="T15" s="11"/>
       <c r="U15" s="56"/>
       <c r="V15" s="57"/>
       <c r="W15" s="58"/>
@@ -2555,7 +2563,7 @@
       <c r="O16" s="54"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="55"/>
-      <c r="T16" s="10"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="56"/>
       <c r="V16" s="57"/>
       <c r="W16" s="58"/>
@@ -2588,7 +2596,7 @@
       <c r="O17" s="54"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="55"/>
-      <c r="T17" s="10"/>
+      <c r="T17" s="11"/>
       <c r="U17" s="56"/>
       <c r="V17" s="57"/>
       <c r="W17" s="58"/>
@@ -2621,7 +2629,7 @@
       <c r="O18" s="54"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="55"/>
-      <c r="T18" s="10"/>
+      <c r="T18" s="11"/>
       <c r="U18" s="56"/>
       <c r="V18" s="57"/>
       <c r="W18" s="58"/>
@@ -2654,7 +2662,7 @@
       <c r="O19" s="54"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="55"/>
-      <c r="T19" s="10"/>
+      <c r="T19" s="11"/>
       <c r="U19" s="56"/>
       <c r="V19" s="57"/>
       <c r="W19" s="58"/>
@@ -2687,7 +2695,7 @@
       <c r="O20" s="54"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="55"/>
-      <c r="T20" s="10"/>
+      <c r="T20" s="11"/>
       <c r="U20" s="56"/>
       <c r="V20" s="57"/>
       <c r="W20" s="58"/>
@@ -2720,7 +2728,7 @@
       <c r="O21" s="54"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="55"/>
-      <c r="T21" s="10"/>
+      <c r="T21" s="11"/>
       <c r="U21" s="56"/>
       <c r="V21" s="57"/>
       <c r="W21" s="58"/>
@@ -2753,7 +2761,7 @@
       <c r="O22" s="54"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="55"/>
-      <c r="T22" s="10"/>
+      <c r="T22" s="11"/>
       <c r="U22" s="56"/>
       <c r="V22" s="57"/>
       <c r="W22" s="58"/>
@@ -2786,7 +2794,7 @@
       <c r="O23" s="54"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="55"/>
-      <c r="T23" s="10"/>
+      <c r="T23" s="11"/>
       <c r="U23" s="56"/>
       <c r="V23" s="57"/>
       <c r="W23" s="58"/>
@@ -2819,7 +2827,7 @@
       <c r="O24" s="54"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="55"/>
-      <c r="T24" s="10"/>
+      <c r="T24" s="11"/>
       <c r="U24" s="56"/>
       <c r="V24" s="57"/>
       <c r="W24" s="58"/>
@@ -2852,7 +2860,7 @@
       <c r="O25" s="54"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="55"/>
-      <c r="T25" s="10"/>
+      <c r="T25" s="11"/>
       <c r="U25" s="56"/>
       <c r="V25" s="57"/>
       <c r="W25" s="58"/>
@@ -2885,7 +2893,7 @@
       <c r="O26" s="54"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="55"/>
-      <c r="T26" s="10"/>
+      <c r="T26" s="11"/>
       <c r="U26" s="56"/>
       <c r="V26" s="57"/>
       <c r="W26" s="58"/>
@@ -2918,7 +2926,7 @@
       <c r="O27" s="54"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="55"/>
-      <c r="T27" s="10"/>
+      <c r="T27" s="11"/>
       <c r="U27" s="56"/>
       <c r="V27" s="57"/>
       <c r="W27" s="58"/>
@@ -2951,7 +2959,7 @@
       <c r="O28" s="54"/>
       <c r="P28" s="29"/>
       <c r="Q28" s="55"/>
-      <c r="T28" s="10"/>
+      <c r="T28" s="11"/>
       <c r="U28" s="56"/>
       <c r="V28" s="57"/>
       <c r="W28" s="58"/>
@@ -2984,7 +2992,7 @@
       <c r="O29" s="54"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="55"/>
-      <c r="T29" s="10"/>
+      <c r="T29" s="11"/>
       <c r="U29" s="56"/>
       <c r="V29" s="57"/>
       <c r="W29" s="58"/>
@@ -3017,7 +3025,7 @@
       <c r="O30" s="54"/>
       <c r="P30" s="29"/>
       <c r="Q30" s="55"/>
-      <c r="T30" s="10"/>
+      <c r="T30" s="11"/>
       <c r="U30" s="56"/>
       <c r="V30" s="57"/>
       <c r="W30" s="58"/>
@@ -3050,7 +3058,7 @@
       <c r="O31" s="54"/>
       <c r="P31" s="29"/>
       <c r="Q31" s="55"/>
-      <c r="T31" s="10"/>
+      <c r="T31" s="11"/>
       <c r="U31" s="56"/>
       <c r="V31" s="57"/>
       <c r="W31" s="58"/>
@@ -3083,7 +3091,7 @@
       <c r="O32" s="54"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="55"/>
-      <c r="T32" s="10"/>
+      <c r="T32" s="11"/>
       <c r="U32" s="56"/>
       <c r="V32" s="57"/>
       <c r="W32" s="58"/>
@@ -3116,7 +3124,7 @@
       <c r="O33" s="54"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="55"/>
-      <c r="T33" s="10"/>
+      <c r="T33" s="11"/>
       <c r="U33" s="56"/>
       <c r="V33" s="57"/>
       <c r="W33" s="58"/>
@@ -3149,7 +3157,7 @@
       <c r="O34" s="54"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="55"/>
-      <c r="T34" s="10"/>
+      <c r="T34" s="11"/>
       <c r="U34" s="56"/>
       <c r="V34" s="57"/>
       <c r="W34" s="58"/>
@@ -3182,7 +3190,7 @@
       <c r="O35" s="54"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="55"/>
-      <c r="T35" s="10"/>
+      <c r="T35" s="11"/>
       <c r="U35" s="56"/>
       <c r="V35" s="57"/>
       <c r="W35" s="58"/>
@@ -3215,7 +3223,7 @@
       <c r="O36" s="54"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="55"/>
-      <c r="T36" s="10"/>
+      <c r="T36" s="11"/>
       <c r="U36" s="56"/>
       <c r="V36" s="57"/>
       <c r="W36" s="58"/>
@@ -3248,7 +3256,7 @@
       <c r="O37" s="54"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="55"/>
-      <c r="T37" s="10"/>
+      <c r="T37" s="11"/>
       <c r="U37" s="56"/>
       <c r="V37" s="57"/>
       <c r="W37" s="58"/>
@@ -3281,7 +3289,7 @@
       <c r="O38" s="54"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="55"/>
-      <c r="T38" s="10"/>
+      <c r="T38" s="11"/>
       <c r="U38" s="56"/>
       <c r="V38" s="57"/>
       <c r="W38" s="58"/>
@@ -3314,7 +3322,7 @@
       <c r="O39" s="54"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="55"/>
-      <c r="T39" s="10"/>
+      <c r="T39" s="11"/>
       <c r="U39" s="56"/>
       <c r="V39" s="57"/>
       <c r="W39" s="58"/>
@@ -3347,7 +3355,7 @@
       <c r="O40" s="54"/>
       <c r="P40" s="29"/>
       <c r="Q40" s="55"/>
-      <c r="T40" s="10"/>
+      <c r="T40" s="11"/>
       <c r="U40" s="56"/>
       <c r="V40" s="57"/>
       <c r="W40" s="58"/>
@@ -3380,7 +3388,7 @@
       <c r="O41" s="54"/>
       <c r="P41" s="29"/>
       <c r="Q41" s="55"/>
-      <c r="T41" s="10"/>
+      <c r="T41" s="11"/>
       <c r="U41" s="56"/>
       <c r="V41" s="57"/>
       <c r="W41" s="58"/>
@@ -3413,7 +3421,7 @@
       <c r="O42" s="54"/>
       <c r="P42" s="29"/>
       <c r="Q42" s="55"/>
-      <c r="T42" s="10"/>
+      <c r="T42" s="11"/>
       <c r="U42" s="56"/>
       <c r="V42" s="57"/>
       <c r="W42" s="58"/>
@@ -3446,7 +3454,7 @@
       <c r="O43" s="54"/>
       <c r="P43" s="29"/>
       <c r="Q43" s="55"/>
-      <c r="T43" s="10"/>
+      <c r="T43" s="11"/>
       <c r="U43" s="56"/>
       <c r="V43" s="57"/>
       <c r="W43" s="58"/>
@@ -3479,7 +3487,7 @@
       <c r="O44" s="54"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="55"/>
-      <c r="T44" s="10"/>
+      <c r="T44" s="11"/>
       <c r="U44" s="56"/>
       <c r="V44" s="57"/>
       <c r="W44" s="58"/>
@@ -3512,7 +3520,7 @@
       <c r="O45" s="54"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="55"/>
-      <c r="T45" s="10"/>
+      <c r="T45" s="11"/>
       <c r="U45" s="56"/>
       <c r="V45" s="57"/>
       <c r="W45" s="58"/>
@@ -3545,7 +3553,7 @@
       <c r="O46" s="54"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="55"/>
-      <c r="T46" s="10"/>
+      <c r="T46" s="11"/>
       <c r="U46" s="56"/>
       <c r="V46" s="57"/>
       <c r="W46" s="58"/>
@@ -3578,7 +3586,7 @@
       <c r="O47" s="54"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="55"/>
-      <c r="T47" s="10"/>
+      <c r="T47" s="11"/>
       <c r="U47" s="56"/>
       <c r="V47" s="57"/>
       <c r="W47" s="58"/>
@@ -3611,7 +3619,7 @@
       <c r="O48" s="54"/>
       <c r="P48" s="29"/>
       <c r="Q48" s="55"/>
-      <c r="T48" s="10"/>
+      <c r="T48" s="11"/>
       <c r="U48" s="56"/>
       <c r="V48" s="57"/>
       <c r="W48" s="58"/>
@@ -3644,7 +3652,7 @@
       <c r="O49" s="54"/>
       <c r="P49" s="29"/>
       <c r="Q49" s="55"/>
-      <c r="T49" s="10"/>
+      <c r="T49" s="11"/>
       <c r="U49" s="56"/>
       <c r="V49" s="57"/>
       <c r="W49" s="58"/>
@@ -3677,7 +3685,7 @@
       <c r="O50" s="54"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="55"/>
-      <c r="T50" s="10"/>
+      <c r="T50" s="11"/>
       <c r="U50" s="56"/>
       <c r="V50" s="57"/>
       <c r="W50" s="58"/>
@@ -3710,7 +3718,7 @@
       <c r="O51" s="54"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="55"/>
-      <c r="T51" s="10"/>
+      <c r="T51" s="11"/>
       <c r="U51" s="56"/>
       <c r="V51" s="57"/>
       <c r="W51" s="58"/>
@@ -3743,7 +3751,7 @@
       <c r="O52" s="54"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="55"/>
-      <c r="T52" s="10"/>
+      <c r="T52" s="11"/>
       <c r="U52" s="56"/>
       <c r="V52" s="57"/>
       <c r="W52" s="58"/>
@@ -3776,7 +3784,7 @@
       <c r="O53" s="54"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="55"/>
-      <c r="T53" s="10"/>
+      <c r="T53" s="11"/>
       <c r="U53" s="56"/>
       <c r="V53" s="57"/>
       <c r="W53" s="58"/>
@@ -3809,7 +3817,7 @@
       <c r="O54" s="54"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="55"/>
-      <c r="T54" s="10"/>
+      <c r="T54" s="11"/>
       <c r="U54" s="56"/>
       <c r="V54" s="57"/>
       <c r="W54" s="58"/>
@@ -3835,7 +3843,7 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="15">
+  <dataValidations count="16">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -3896,6 +3904,10 @@
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3917,14 +3929,14 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="O43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="AE1" activeCellId="0" sqref="AE1"/>
+      <selection pane="bottomRight" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -3979,7 +3991,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 8</v>
+        <v>Version: 9</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -4003,77 +4015,81 @@
       <c r="M2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="11"/>
+      <c r="N2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="10"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
-      <c r="AA2" s="11"/>
+      <c r="AA2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="10"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
-      <c r="AA3" s="11"/>
+      <c r="AA3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
       <c r="R4" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
       <c r="U4" s="16"/>
       <c r="V4" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W4" s="16"/>
       <c r="X4" s="16"/>
@@ -4081,26 +4097,26 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
       <c r="AB4" s="17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AC4" s="17"/>
       <c r="AD4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>20</v>
@@ -4244,7 +4260,8 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="45" t="b">
+      <c r="Z6" s="45" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AA6" s="46" t="n">
@@ -4278,7 +4295,7 @@
       <c r="O7" s="54"/>
       <c r="P7" s="29"/>
       <c r="Q7" s="55"/>
-      <c r="T7" s="10"/>
+      <c r="T7" s="11"/>
       <c r="U7" s="56"/>
       <c r="V7" s="57"/>
       <c r="W7" s="58"/>
@@ -4311,7 +4328,7 @@
       <c r="O8" s="54"/>
       <c r="P8" s="29"/>
       <c r="Q8" s="55"/>
-      <c r="T8" s="10"/>
+      <c r="T8" s="11"/>
       <c r="U8" s="56"/>
       <c r="V8" s="57"/>
       <c r="W8" s="58"/>
@@ -4344,7 +4361,7 @@
       <c r="O9" s="54"/>
       <c r="P9" s="29"/>
       <c r="Q9" s="55"/>
-      <c r="T9" s="10"/>
+      <c r="T9" s="11"/>
       <c r="U9" s="56"/>
       <c r="V9" s="57"/>
       <c r="W9" s="58"/>
@@ -4377,7 +4394,7 @@
       <c r="O10" s="54"/>
       <c r="P10" s="29"/>
       <c r="Q10" s="55"/>
-      <c r="T10" s="10"/>
+      <c r="T10" s="11"/>
       <c r="U10" s="56"/>
       <c r="V10" s="57"/>
       <c r="W10" s="58"/>
@@ -4410,7 +4427,7 @@
       <c r="O11" s="54"/>
       <c r="P11" s="29"/>
       <c r="Q11" s="55"/>
-      <c r="T11" s="10"/>
+      <c r="T11" s="11"/>
       <c r="U11" s="56"/>
       <c r="V11" s="57"/>
       <c r="W11" s="58"/>
@@ -4443,7 +4460,7 @@
       <c r="O12" s="54"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="55"/>
-      <c r="T12" s="10"/>
+      <c r="T12" s="11"/>
       <c r="U12" s="56"/>
       <c r="V12" s="57"/>
       <c r="W12" s="58"/>
@@ -4476,7 +4493,7 @@
       <c r="O13" s="54"/>
       <c r="P13" s="29"/>
       <c r="Q13" s="55"/>
-      <c r="T13" s="10"/>
+      <c r="T13" s="11"/>
       <c r="U13" s="56"/>
       <c r="V13" s="57"/>
       <c r="W13" s="58"/>
@@ -4509,7 +4526,7 @@
       <c r="O14" s="54"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="55"/>
-      <c r="T14" s="10"/>
+      <c r="T14" s="11"/>
       <c r="U14" s="56"/>
       <c r="V14" s="57"/>
       <c r="W14" s="58"/>
@@ -4542,7 +4559,7 @@
       <c r="O15" s="54"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="55"/>
-      <c r="T15" s="10"/>
+      <c r="T15" s="11"/>
       <c r="U15" s="56"/>
       <c r="V15" s="57"/>
       <c r="W15" s="58"/>
@@ -4575,7 +4592,7 @@
       <c r="O16" s="54"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="55"/>
-      <c r="T16" s="10"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="56"/>
       <c r="V16" s="57"/>
       <c r="W16" s="58"/>
@@ -4608,7 +4625,7 @@
       <c r="O17" s="54"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="55"/>
-      <c r="T17" s="10"/>
+      <c r="T17" s="11"/>
       <c r="U17" s="56"/>
       <c r="V17" s="57"/>
       <c r="W17" s="58"/>
@@ -4641,7 +4658,7 @@
       <c r="O18" s="54"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="55"/>
-      <c r="T18" s="10"/>
+      <c r="T18" s="11"/>
       <c r="U18" s="56"/>
       <c r="V18" s="57"/>
       <c r="W18" s="58"/>
@@ -4674,7 +4691,7 @@
       <c r="O19" s="54"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="55"/>
-      <c r="T19" s="10"/>
+      <c r="T19" s="11"/>
       <c r="U19" s="56"/>
       <c r="V19" s="57"/>
       <c r="W19" s="58"/>
@@ -4707,7 +4724,7 @@
       <c r="O20" s="54"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="55"/>
-      <c r="T20" s="10"/>
+      <c r="T20" s="11"/>
       <c r="U20" s="56"/>
       <c r="V20" s="57"/>
       <c r="W20" s="58"/>
@@ -4740,7 +4757,7 @@
       <c r="O21" s="54"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="55"/>
-      <c r="T21" s="10"/>
+      <c r="T21" s="11"/>
       <c r="U21" s="56"/>
       <c r="V21" s="57"/>
       <c r="W21" s="58"/>
@@ -4773,7 +4790,7 @@
       <c r="O22" s="54"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="55"/>
-      <c r="T22" s="10"/>
+      <c r="T22" s="11"/>
       <c r="U22" s="56"/>
       <c r="V22" s="57"/>
       <c r="W22" s="58"/>
@@ -4806,7 +4823,7 @@
       <c r="O23" s="54"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="55"/>
-      <c r="T23" s="10"/>
+      <c r="T23" s="11"/>
       <c r="U23" s="56"/>
       <c r="V23" s="57"/>
       <c r="W23" s="58"/>
@@ -4839,7 +4856,7 @@
       <c r="O24" s="54"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="55"/>
-      <c r="T24" s="10"/>
+      <c r="T24" s="11"/>
       <c r="U24" s="56"/>
       <c r="V24" s="57"/>
       <c r="W24" s="58"/>
@@ -4872,7 +4889,7 @@
       <c r="O25" s="54"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="55"/>
-      <c r="T25" s="10"/>
+      <c r="T25" s="11"/>
       <c r="U25" s="56"/>
       <c r="V25" s="57"/>
       <c r="W25" s="58"/>
@@ -4905,7 +4922,7 @@
       <c r="O26" s="54"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="55"/>
-      <c r="T26" s="10"/>
+      <c r="T26" s="11"/>
       <c r="U26" s="56"/>
       <c r="V26" s="57"/>
       <c r="W26" s="58"/>
@@ -4938,7 +4955,7 @@
       <c r="O27" s="54"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="55"/>
-      <c r="T27" s="10"/>
+      <c r="T27" s="11"/>
       <c r="U27" s="56"/>
       <c r="V27" s="57"/>
       <c r="W27" s="58"/>
@@ -4971,7 +4988,7 @@
       <c r="O28" s="54"/>
       <c r="P28" s="29"/>
       <c r="Q28" s="55"/>
-      <c r="T28" s="10"/>
+      <c r="T28" s="11"/>
       <c r="U28" s="56"/>
       <c r="V28" s="57"/>
       <c r="W28" s="58"/>
@@ -5004,7 +5021,7 @@
       <c r="O29" s="54"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="55"/>
-      <c r="T29" s="10"/>
+      <c r="T29" s="11"/>
       <c r="U29" s="56"/>
       <c r="V29" s="57"/>
       <c r="W29" s="58"/>
@@ -5037,7 +5054,7 @@
       <c r="O30" s="54"/>
       <c r="P30" s="29"/>
       <c r="Q30" s="55"/>
-      <c r="T30" s="10"/>
+      <c r="T30" s="11"/>
       <c r="U30" s="56"/>
       <c r="V30" s="57"/>
       <c r="W30" s="58"/>
@@ -5070,7 +5087,7 @@
       <c r="O31" s="54"/>
       <c r="P31" s="29"/>
       <c r="Q31" s="55"/>
-      <c r="T31" s="10"/>
+      <c r="T31" s="11"/>
       <c r="U31" s="56"/>
       <c r="V31" s="57"/>
       <c r="W31" s="58"/>
@@ -5103,7 +5120,7 @@
       <c r="O32" s="54"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="55"/>
-      <c r="T32" s="10"/>
+      <c r="T32" s="11"/>
       <c r="U32" s="56"/>
       <c r="V32" s="57"/>
       <c r="W32" s="58"/>
@@ -5136,7 +5153,7 @@
       <c r="O33" s="54"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="55"/>
-      <c r="T33" s="10"/>
+      <c r="T33" s="11"/>
       <c r="U33" s="56"/>
       <c r="V33" s="57"/>
       <c r="W33" s="58"/>
@@ -5169,7 +5186,7 @@
       <c r="O34" s="54"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="55"/>
-      <c r="T34" s="10"/>
+      <c r="T34" s="11"/>
       <c r="U34" s="56"/>
       <c r="V34" s="57"/>
       <c r="W34" s="58"/>
@@ -5202,7 +5219,7 @@
       <c r="O35" s="54"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="55"/>
-      <c r="T35" s="10"/>
+      <c r="T35" s="11"/>
       <c r="U35" s="56"/>
       <c r="V35" s="57"/>
       <c r="W35" s="58"/>
@@ -5235,7 +5252,7 @@
       <c r="O36" s="54"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="55"/>
-      <c r="T36" s="10"/>
+      <c r="T36" s="11"/>
       <c r="U36" s="56"/>
       <c r="V36" s="57"/>
       <c r="W36" s="58"/>
@@ -5268,7 +5285,7 @@
       <c r="O37" s="54"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="55"/>
-      <c r="T37" s="10"/>
+      <c r="T37" s="11"/>
       <c r="U37" s="56"/>
       <c r="V37" s="57"/>
       <c r="W37" s="58"/>
@@ -5301,7 +5318,7 @@
       <c r="O38" s="54"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="55"/>
-      <c r="T38" s="10"/>
+      <c r="T38" s="11"/>
       <c r="U38" s="56"/>
       <c r="V38" s="57"/>
       <c r="W38" s="58"/>
@@ -5334,7 +5351,7 @@
       <c r="O39" s="54"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="55"/>
-      <c r="T39" s="10"/>
+      <c r="T39" s="11"/>
       <c r="U39" s="56"/>
       <c r="V39" s="57"/>
       <c r="W39" s="58"/>
@@ -5367,7 +5384,7 @@
       <c r="O40" s="54"/>
       <c r="P40" s="29"/>
       <c r="Q40" s="55"/>
-      <c r="T40" s="10"/>
+      <c r="T40" s="11"/>
       <c r="U40" s="56"/>
       <c r="V40" s="57"/>
       <c r="W40" s="58"/>
@@ -5400,7 +5417,7 @@
       <c r="O41" s="54"/>
       <c r="P41" s="29"/>
       <c r="Q41" s="55"/>
-      <c r="T41" s="10"/>
+      <c r="T41" s="11"/>
       <c r="U41" s="56"/>
       <c r="V41" s="57"/>
       <c r="W41" s="58"/>
@@ -5433,7 +5450,7 @@
       <c r="O42" s="54"/>
       <c r="P42" s="29"/>
       <c r="Q42" s="55"/>
-      <c r="T42" s="10"/>
+      <c r="T42" s="11"/>
       <c r="U42" s="56"/>
       <c r="V42" s="57"/>
       <c r="W42" s="58"/>
@@ -5466,7 +5483,7 @@
       <c r="O43" s="54"/>
       <c r="P43" s="29"/>
       <c r="Q43" s="55"/>
-      <c r="T43" s="10"/>
+      <c r="T43" s="11"/>
       <c r="U43" s="56"/>
       <c r="V43" s="57"/>
       <c r="W43" s="58"/>
@@ -5499,7 +5516,7 @@
       <c r="O44" s="54"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="55"/>
-      <c r="T44" s="10"/>
+      <c r="T44" s="11"/>
       <c r="U44" s="56"/>
       <c r="V44" s="57"/>
       <c r="W44" s="58"/>
@@ -5532,7 +5549,7 @@
       <c r="O45" s="54"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="55"/>
-      <c r="T45" s="10"/>
+      <c r="T45" s="11"/>
       <c r="U45" s="56"/>
       <c r="V45" s="57"/>
       <c r="W45" s="58"/>
@@ -5565,7 +5582,7 @@
       <c r="O46" s="54"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="55"/>
-      <c r="T46" s="10"/>
+      <c r="T46" s="11"/>
       <c r="U46" s="56"/>
       <c r="V46" s="57"/>
       <c r="W46" s="58"/>
@@ -5598,7 +5615,7 @@
       <c r="O47" s="54"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="55"/>
-      <c r="T47" s="10"/>
+      <c r="T47" s="11"/>
       <c r="U47" s="56"/>
       <c r="V47" s="57"/>
       <c r="W47" s="58"/>
@@ -5631,7 +5648,7 @@
       <c r="O48" s="54"/>
       <c r="P48" s="29"/>
       <c r="Q48" s="55"/>
-      <c r="T48" s="10"/>
+      <c r="T48" s="11"/>
       <c r="U48" s="56"/>
       <c r="V48" s="57"/>
       <c r="W48" s="58"/>
@@ -5664,7 +5681,7 @@
       <c r="O49" s="54"/>
       <c r="P49" s="29"/>
       <c r="Q49" s="55"/>
-      <c r="T49" s="10"/>
+      <c r="T49" s="11"/>
       <c r="U49" s="56"/>
       <c r="V49" s="57"/>
       <c r="W49" s="58"/>
@@ -5697,7 +5714,7 @@
       <c r="O50" s="54"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="55"/>
-      <c r="T50" s="10"/>
+      <c r="T50" s="11"/>
       <c r="U50" s="56"/>
       <c r="V50" s="57"/>
       <c r="W50" s="58"/>
@@ -5730,7 +5747,7 @@
       <c r="O51" s="54"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="55"/>
-      <c r="T51" s="10"/>
+      <c r="T51" s="11"/>
       <c r="U51" s="56"/>
       <c r="V51" s="57"/>
       <c r="W51" s="58"/>
@@ -5763,7 +5780,7 @@
       <c r="O52" s="54"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="55"/>
-      <c r="T52" s="10"/>
+      <c r="T52" s="11"/>
       <c r="U52" s="56"/>
       <c r="V52" s="57"/>
       <c r="W52" s="58"/>
@@ -5796,7 +5813,7 @@
       <c r="O53" s="54"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="55"/>
-      <c r="T53" s="10"/>
+      <c r="T53" s="11"/>
       <c r="U53" s="56"/>
       <c r="V53" s="57"/>
       <c r="W53" s="58"/>
@@ -5829,7 +5846,7 @@
       <c r="O54" s="54"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="55"/>
-      <c r="T54" s="10"/>
+      <c r="T54" s="11"/>
       <c r="U54" s="56"/>
       <c r="V54" s="57"/>
       <c r="W54" s="58"/>
@@ -5855,7 +5872,7 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="15">
+  <dataValidations count="16">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -5916,6 +5933,10 @@
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5936,15 +5957,15 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="AE1" activeCellId="0" sqref="AE1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -5999,7 +6020,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 8</v>
+        <v>Version: 9</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -6023,77 +6044,81 @@
       <c r="M2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="11"/>
+      <c r="N2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="10"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
-      <c r="AA2" s="11"/>
+      <c r="AA2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="10"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
-      <c r="AA3" s="11"/>
+      <c r="AA3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
       <c r="R4" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
       <c r="U4" s="16"/>
       <c r="V4" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W4" s="16"/>
       <c r="X4" s="16"/>
@@ -6101,26 +6126,26 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
       <c r="AB4" s="17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AC4" s="17"/>
       <c r="AD4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>20</v>
@@ -6264,7 +6289,8 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="45" t="b">
+      <c r="Z6" s="45" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AA6" s="46" t="n">
@@ -6298,7 +6324,7 @@
       <c r="O7" s="54"/>
       <c r="P7" s="29"/>
       <c r="Q7" s="55"/>
-      <c r="T7" s="10"/>
+      <c r="T7" s="11"/>
       <c r="U7" s="56"/>
       <c r="V7" s="57"/>
       <c r="W7" s="58"/>
@@ -6331,7 +6357,7 @@
       <c r="O8" s="54"/>
       <c r="P8" s="29"/>
       <c r="Q8" s="55"/>
-      <c r="T8" s="10"/>
+      <c r="T8" s="11"/>
       <c r="U8" s="56"/>
       <c r="V8" s="57"/>
       <c r="W8" s="58"/>
@@ -6364,7 +6390,7 @@
       <c r="O9" s="54"/>
       <c r="P9" s="29"/>
       <c r="Q9" s="55"/>
-      <c r="T9" s="10"/>
+      <c r="T9" s="11"/>
       <c r="U9" s="56"/>
       <c r="V9" s="57"/>
       <c r="W9" s="58"/>
@@ -6397,7 +6423,7 @@
       <c r="O10" s="54"/>
       <c r="P10" s="29"/>
       <c r="Q10" s="55"/>
-      <c r="T10" s="10"/>
+      <c r="T10" s="11"/>
       <c r="U10" s="56"/>
       <c r="V10" s="57"/>
       <c r="W10" s="58"/>
@@ -6430,7 +6456,7 @@
       <c r="O11" s="54"/>
       <c r="P11" s="29"/>
       <c r="Q11" s="55"/>
-      <c r="T11" s="10"/>
+      <c r="T11" s="11"/>
       <c r="U11" s="56"/>
       <c r="V11" s="57"/>
       <c r="W11" s="58"/>
@@ -6463,7 +6489,7 @@
       <c r="O12" s="54"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="55"/>
-      <c r="T12" s="10"/>
+      <c r="T12" s="11"/>
       <c r="U12" s="56"/>
       <c r="V12" s="57"/>
       <c r="W12" s="58"/>
@@ -6496,7 +6522,7 @@
       <c r="O13" s="54"/>
       <c r="P13" s="29"/>
       <c r="Q13" s="55"/>
-      <c r="T13" s="10"/>
+      <c r="T13" s="11"/>
       <c r="U13" s="56"/>
       <c r="V13" s="57"/>
       <c r="W13" s="58"/>
@@ -6529,7 +6555,7 @@
       <c r="O14" s="54"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="55"/>
-      <c r="T14" s="10"/>
+      <c r="T14" s="11"/>
       <c r="U14" s="56"/>
       <c r="V14" s="57"/>
       <c r="W14" s="58"/>
@@ -6562,7 +6588,7 @@
       <c r="O15" s="54"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="55"/>
-      <c r="T15" s="10"/>
+      <c r="T15" s="11"/>
       <c r="U15" s="56"/>
       <c r="V15" s="57"/>
       <c r="W15" s="58"/>
@@ -6595,7 +6621,7 @@
       <c r="O16" s="54"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="55"/>
-      <c r="T16" s="10"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="56"/>
       <c r="V16" s="57"/>
       <c r="W16" s="58"/>
@@ -6628,7 +6654,7 @@
       <c r="O17" s="54"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="55"/>
-      <c r="T17" s="10"/>
+      <c r="T17" s="11"/>
       <c r="U17" s="56"/>
       <c r="V17" s="57"/>
       <c r="W17" s="58"/>
@@ -6661,7 +6687,7 @@
       <c r="O18" s="54"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="55"/>
-      <c r="T18" s="10"/>
+      <c r="T18" s="11"/>
       <c r="U18" s="56"/>
       <c r="V18" s="57"/>
       <c r="W18" s="58"/>
@@ -6694,7 +6720,7 @@
       <c r="O19" s="54"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="55"/>
-      <c r="T19" s="10"/>
+      <c r="T19" s="11"/>
       <c r="U19" s="56"/>
       <c r="V19" s="57"/>
       <c r="W19" s="58"/>
@@ -6727,7 +6753,7 @@
       <c r="O20" s="54"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="55"/>
-      <c r="T20" s="10"/>
+      <c r="T20" s="11"/>
       <c r="U20" s="56"/>
       <c r="V20" s="57"/>
       <c r="W20" s="58"/>
@@ -6760,7 +6786,7 @@
       <c r="O21" s="54"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="55"/>
-      <c r="T21" s="10"/>
+      <c r="T21" s="11"/>
       <c r="U21" s="56"/>
       <c r="V21" s="57"/>
       <c r="W21" s="58"/>
@@ -6793,7 +6819,7 @@
       <c r="O22" s="54"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="55"/>
-      <c r="T22" s="10"/>
+      <c r="T22" s="11"/>
       <c r="U22" s="56"/>
       <c r="V22" s="57"/>
       <c r="W22" s="58"/>
@@ -6826,7 +6852,7 @@
       <c r="O23" s="54"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="55"/>
-      <c r="T23" s="10"/>
+      <c r="T23" s="11"/>
       <c r="U23" s="56"/>
       <c r="V23" s="57"/>
       <c r="W23" s="58"/>
@@ -6859,7 +6885,7 @@
       <c r="O24" s="54"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="55"/>
-      <c r="T24" s="10"/>
+      <c r="T24" s="11"/>
       <c r="U24" s="56"/>
       <c r="V24" s="57"/>
       <c r="W24" s="58"/>
@@ -6892,7 +6918,7 @@
       <c r="O25" s="54"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="55"/>
-      <c r="T25" s="10"/>
+      <c r="T25" s="11"/>
       <c r="U25" s="56"/>
       <c r="V25" s="57"/>
       <c r="W25" s="58"/>
@@ -6925,7 +6951,7 @@
       <c r="O26" s="54"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="55"/>
-      <c r="T26" s="10"/>
+      <c r="T26" s="11"/>
       <c r="U26" s="56"/>
       <c r="V26" s="57"/>
       <c r="W26" s="58"/>
@@ -6958,7 +6984,7 @@
       <c r="O27" s="54"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="55"/>
-      <c r="T27" s="10"/>
+      <c r="T27" s="11"/>
       <c r="U27" s="56"/>
       <c r="V27" s="57"/>
       <c r="W27" s="58"/>
@@ -6991,7 +7017,7 @@
       <c r="O28" s="54"/>
       <c r="P28" s="29"/>
       <c r="Q28" s="55"/>
-      <c r="T28" s="10"/>
+      <c r="T28" s="11"/>
       <c r="U28" s="56"/>
       <c r="V28" s="57"/>
       <c r="W28" s="58"/>
@@ -7024,7 +7050,7 @@
       <c r="O29" s="54"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="55"/>
-      <c r="T29" s="10"/>
+      <c r="T29" s="11"/>
       <c r="U29" s="56"/>
       <c r="V29" s="57"/>
       <c r="W29" s="58"/>
@@ -7057,7 +7083,7 @@
       <c r="O30" s="54"/>
       <c r="P30" s="29"/>
       <c r="Q30" s="55"/>
-      <c r="T30" s="10"/>
+      <c r="T30" s="11"/>
       <c r="U30" s="56"/>
       <c r="V30" s="57"/>
       <c r="W30" s="58"/>
@@ -7090,7 +7116,7 @@
       <c r="O31" s="54"/>
       <c r="P31" s="29"/>
       <c r="Q31" s="55"/>
-      <c r="T31" s="10"/>
+      <c r="T31" s="11"/>
       <c r="U31" s="56"/>
       <c r="V31" s="57"/>
       <c r="W31" s="58"/>
@@ -7123,7 +7149,7 @@
       <c r="O32" s="54"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="55"/>
-      <c r="T32" s="10"/>
+      <c r="T32" s="11"/>
       <c r="U32" s="56"/>
       <c r="V32" s="57"/>
       <c r="W32" s="58"/>
@@ -7156,7 +7182,7 @@
       <c r="O33" s="54"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="55"/>
-      <c r="T33" s="10"/>
+      <c r="T33" s="11"/>
       <c r="U33" s="56"/>
       <c r="V33" s="57"/>
       <c r="W33" s="58"/>
@@ -7189,7 +7215,7 @@
       <c r="O34" s="54"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="55"/>
-      <c r="T34" s="10"/>
+      <c r="T34" s="11"/>
       <c r="U34" s="56"/>
       <c r="V34" s="57"/>
       <c r="W34" s="58"/>
@@ -7222,7 +7248,7 @@
       <c r="O35" s="54"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="55"/>
-      <c r="T35" s="10"/>
+      <c r="T35" s="11"/>
       <c r="U35" s="56"/>
       <c r="V35" s="57"/>
       <c r="W35" s="58"/>
@@ -7255,7 +7281,7 @@
       <c r="O36" s="54"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="55"/>
-      <c r="T36" s="10"/>
+      <c r="T36" s="11"/>
       <c r="U36" s="56"/>
       <c r="V36" s="57"/>
       <c r="W36" s="58"/>
@@ -7288,7 +7314,7 @@
       <c r="O37" s="54"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="55"/>
-      <c r="T37" s="10"/>
+      <c r="T37" s="11"/>
       <c r="U37" s="56"/>
       <c r="V37" s="57"/>
       <c r="W37" s="58"/>
@@ -7321,7 +7347,7 @@
       <c r="O38" s="54"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="55"/>
-      <c r="T38" s="10"/>
+      <c r="T38" s="11"/>
       <c r="U38" s="56"/>
       <c r="V38" s="57"/>
       <c r="W38" s="58"/>
@@ -7354,7 +7380,7 @@
       <c r="O39" s="54"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="55"/>
-      <c r="T39" s="10"/>
+      <c r="T39" s="11"/>
       <c r="U39" s="56"/>
       <c r="V39" s="57"/>
       <c r="W39" s="58"/>
@@ -7387,7 +7413,7 @@
       <c r="O40" s="54"/>
       <c r="P40" s="29"/>
       <c r="Q40" s="55"/>
-      <c r="T40" s="10"/>
+      <c r="T40" s="11"/>
       <c r="U40" s="56"/>
       <c r="V40" s="57"/>
       <c r="W40" s="58"/>
@@ -7420,7 +7446,7 @@
       <c r="O41" s="54"/>
       <c r="P41" s="29"/>
       <c r="Q41" s="55"/>
-      <c r="T41" s="10"/>
+      <c r="T41" s="11"/>
       <c r="U41" s="56"/>
       <c r="V41" s="57"/>
       <c r="W41" s="58"/>
@@ -7453,7 +7479,7 @@
       <c r="O42" s="54"/>
       <c r="P42" s="29"/>
       <c r="Q42" s="55"/>
-      <c r="T42" s="10"/>
+      <c r="T42" s="11"/>
       <c r="U42" s="56"/>
       <c r="V42" s="57"/>
       <c r="W42" s="58"/>
@@ -7486,7 +7512,7 @@
       <c r="O43" s="54"/>
       <c r="P43" s="29"/>
       <c r="Q43" s="55"/>
-      <c r="T43" s="10"/>
+      <c r="T43" s="11"/>
       <c r="U43" s="56"/>
       <c r="V43" s="57"/>
       <c r="W43" s="58"/>
@@ -7519,7 +7545,7 @@
       <c r="O44" s="54"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="55"/>
-      <c r="T44" s="10"/>
+      <c r="T44" s="11"/>
       <c r="U44" s="56"/>
       <c r="V44" s="57"/>
       <c r="W44" s="58"/>
@@ -7552,7 +7578,7 @@
       <c r="O45" s="54"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="55"/>
-      <c r="T45" s="10"/>
+      <c r="T45" s="11"/>
       <c r="U45" s="56"/>
       <c r="V45" s="57"/>
       <c r="W45" s="58"/>
@@ -7585,7 +7611,7 @@
       <c r="O46" s="54"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="55"/>
-      <c r="T46" s="10"/>
+      <c r="T46" s="11"/>
       <c r="U46" s="56"/>
       <c r="V46" s="57"/>
       <c r="W46" s="58"/>
@@ -7618,7 +7644,7 @@
       <c r="O47" s="54"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="55"/>
-      <c r="T47" s="10"/>
+      <c r="T47" s="11"/>
       <c r="U47" s="56"/>
       <c r="V47" s="57"/>
       <c r="W47" s="58"/>
@@ -7651,7 +7677,7 @@
       <c r="O48" s="54"/>
       <c r="P48" s="29"/>
       <c r="Q48" s="55"/>
-      <c r="T48" s="10"/>
+      <c r="T48" s="11"/>
       <c r="U48" s="56"/>
       <c r="V48" s="57"/>
       <c r="W48" s="58"/>
@@ -7684,7 +7710,7 @@
       <c r="O49" s="54"/>
       <c r="P49" s="29"/>
       <c r="Q49" s="55"/>
-      <c r="T49" s="10"/>
+      <c r="T49" s="11"/>
       <c r="U49" s="56"/>
       <c r="V49" s="57"/>
       <c r="W49" s="58"/>
@@ -7717,7 +7743,7 @@
       <c r="O50" s="54"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="55"/>
-      <c r="T50" s="10"/>
+      <c r="T50" s="11"/>
       <c r="U50" s="56"/>
       <c r="V50" s="57"/>
       <c r="W50" s="58"/>
@@ -7750,7 +7776,7 @@
       <c r="O51" s="54"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="55"/>
-      <c r="T51" s="10"/>
+      <c r="T51" s="11"/>
       <c r="U51" s="56"/>
       <c r="V51" s="57"/>
       <c r="W51" s="58"/>
@@ -7783,7 +7809,7 @@
       <c r="O52" s="54"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="55"/>
-      <c r="T52" s="10"/>
+      <c r="T52" s="11"/>
       <c r="U52" s="56"/>
       <c r="V52" s="57"/>
       <c r="W52" s="58"/>
@@ -7816,7 +7842,7 @@
       <c r="O53" s="54"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="55"/>
-      <c r="T53" s="10"/>
+      <c r="T53" s="11"/>
       <c r="U53" s="56"/>
       <c r="V53" s="57"/>
       <c r="W53" s="58"/>
@@ -7849,7 +7875,7 @@
       <c r="O54" s="54"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="55"/>
-      <c r="T54" s="10"/>
+      <c r="T54" s="11"/>
       <c r="U54" s="56"/>
       <c r="V54" s="57"/>
       <c r="W54" s="58"/>
@@ -7875,7 +7901,7 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="15">
+  <dataValidations count="16">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -7936,6 +7962,10 @@
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7954,13 +7984,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -7979,7 +8009,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="61"/>
     </row>
@@ -8057,6 +8087,14 @@
       </c>
       <c r="B13" s="0" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clarified non-use of default row for motor positions in automation spreadsheets
</commit_message>
<xml_diff>
--- a/startup/xlsx/doublewheel.xlsx
+++ b/startup/xlsx/doublewheel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="dw1" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -54,6 +54,62 @@
         </r>
       </text>
     </comment>
+    <comment ref="R6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -61,7 +117,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -90,6 +146,62 @@
         </r>
       </text>
     </comment>
+    <comment ref="R6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -97,7 +209,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -123,6 +235,62 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
         </r>
       </text>
     </comment>
@@ -620,8 +788,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border diagonalUp="true" diagonalDown="true">
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
       <right style="thin"/>
       <top style="thin">
         <color rgb="FFCCCCCC"/>
@@ -629,7 +799,7 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="medium"/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
@@ -1000,9 +1170,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
+      <xdr:colOff>93600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1011,8 +1181,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3356280" y="10725120"/>
-          <a:ext cx="6648120" cy="2259000"/>
+          <a:off x="3357000" y="10725120"/>
+          <a:ext cx="6648120" cy="2258640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1259,9 +1429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098000</xdr:colOff>
+      <xdr:colOff>1097640</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1274,13 +1444,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1299600" y="10772280"/>
-          <a:ext cx="1833480" cy="2445840"/>
+          <a:off x="1300320" y="10772280"/>
+          <a:ext cx="1833120" cy="2445480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1301,9 +1471,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
+      <xdr:colOff>93600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1312,8 +1482,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3356280" y="10725120"/>
-          <a:ext cx="6648120" cy="2259000"/>
+          <a:off x="3357000" y="10725120"/>
+          <a:ext cx="6648120" cy="2258640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1560,9 +1730,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098000</xdr:colOff>
+      <xdr:colOff>1097640</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1575,13 +1745,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1299600" y="10772280"/>
-          <a:ext cx="1833480" cy="2445840"/>
+          <a:off x="1300320" y="10772280"/>
+          <a:ext cx="1833120" cy="2445480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1602,9 +1772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
+      <xdr:colOff>93600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1613,8 +1783,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3356280" y="10725120"/>
-          <a:ext cx="6648120" cy="2259000"/>
+          <a:off x="3357000" y="10725120"/>
+          <a:ext cx="6648120" cy="2258640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1861,9 +2031,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098000</xdr:colOff>
+      <xdr:colOff>1097640</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1876,13 +2046,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1299600" y="10772280"/>
-          <a:ext cx="1833480" cy="2445840"/>
+          <a:off x="1300320" y="10772280"/>
+          <a:ext cx="1833120" cy="2445480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1899,15 +2069,15 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -2212,9 +2382,9 @@
         <v>57</v>
       </c>
       <c r="R6" s="43"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
       <c r="V6" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
@@ -3844,74 +4014,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3933,10 +4103,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -4241,9 +4411,9 @@
         <v>57</v>
       </c>
       <c r="R6" s="43"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
       <c r="V6" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
@@ -5873,74 +6043,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5962,10 +6132,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -6270,9 +6440,9 @@
         <v>57</v>
       </c>
       <c r="R6" s="43"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
       <c r="V6" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
@@ -7902,74 +8072,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -7986,11 +8156,11 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -8100,7 +8270,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
usbstick defaults to false in all spredsheets
</commit_message>
<xml_diff>
--- a/startup/xlsx/doublewheel.xlsx
+++ b/startup/xlsx/doublewheel.xlsx
@@ -1173,9 +1173,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93240</xdr:colOff>
+      <xdr:colOff>92880</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1184,8 +1184,309 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3357720" y="10725120"/>
-          <a:ext cx="6648480" cy="2258280"/>
+          <a:off x="3358440" y="10725120"/>
+          <a:ext cx="6648480" cy="2257920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="73080">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFillTx/>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>Instructions:</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>2. Default values for all parameters go in line 6</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Specify detector position in column U, blank means to </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>not move</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t> the detector </a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Do not add rows above row 7</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>7. Do not add columns before column AE</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>8. The wheel is correctly mounted if the numbers can be read when facing the wheel</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>677160</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>42840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>49320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1301760" y="10772280"/>
+          <a:ext cx="1832400" cy="2444760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66600</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>92880</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>140400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3358440" y="10725120"/>
+          <a:ext cx="6648480" cy="2257920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1432,13 +1733,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:colOff>1096920</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPr id="3" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1447,8 +1748,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1300680" y="10772280"/>
-          <a:ext cx="1832760" cy="2445120"/>
+          <a:off x="1301400" y="10772280"/>
+          <a:ext cx="1832400" cy="2444760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1463,7 +1764,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
@@ -1474,19 +1775,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93240</xdr:colOff>
+      <xdr:colOff>92880</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3357720" y="10725120"/>
-          <a:ext cx="6648480" cy="2258280"/>
+          <a:off x="3358440" y="10725120"/>
+          <a:ext cx="6648480" cy="2257920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1733,310 +2034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:colOff>1096920</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1300680" y="10772280"/>
-          <a:ext cx="1832760" cy="2445120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>93240</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3357720" y="10725120"/>
-          <a:ext cx="6648480" cy="2258280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="73080">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>Instructions:</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>2. Default values for all parameters go in line 6</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Specify detector position in column U, blank means to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>not move</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t> the detector </a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Do not add rows above row 7</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>7. Do not add columns before column AE</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>8. The wheel is correctly mounted if the numbers can be read when facing the wheel</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>676800</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2049,8 +2049,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1300680" y="10772280"/>
-          <a:ext cx="1832760" cy="2445120"/>
+          <a:off x="1301400" y="10772280"/>
+          <a:ext cx="1832400" cy="2444760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2073,14 +2073,14 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -2397,8 +2397,8 @@
         <v>1</v>
       </c>
       <c r="X6" s="45" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="Y6" s="45" t="n">
         <f aca="false">FALSE()</f>
@@ -4102,14 +4102,14 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -4426,8 +4426,8 @@
         <v>1</v>
       </c>
       <c r="X6" s="45" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="Y6" s="45" t="n">
         <f aca="false">FALSE()</f>
@@ -6135,10 +6135,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -6455,8 +6455,8 @@
         <v>1</v>
       </c>
       <c r="X6" s="45" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="Y6" s="45" t="n">
         <f aca="false">FALSE()</f>
@@ -8163,7 +8163,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>

</xml_diff>

<commit_message>
added a thrid motor column to grid spreadsheet
</commit_message>
<xml_diff>
--- a/startup/xlsx/doublewheel.xlsx
+++ b/startup/xlsx/doublewheel.xlsx
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="73">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -515,6 +515,9 @@
   </si>
   <si>
     <t xml:space="preserve">add slit height to glancing angle spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add a third motor to the grid spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -1173,9 +1176,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92880</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1184,8 +1187,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358440" y="10725120"/>
-          <a:ext cx="6648480" cy="2257920"/>
+          <a:off x="3358800" y="10725120"/>
+          <a:ext cx="6649200" cy="2257560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1432,9 +1435,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:colOff>1096920</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1447,8 +1450,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1301760" y="10772280"/>
-          <a:ext cx="1832400" cy="2444760"/>
+          <a:off x="1302480" y="10772280"/>
+          <a:ext cx="1832040" cy="2444400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1474,9 +1477,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92880</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1485,8 +1488,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358440" y="10725120"/>
-          <a:ext cx="6648480" cy="2257920"/>
+          <a:off x="3358800" y="10725120"/>
+          <a:ext cx="6649200" cy="2257560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1733,9 +1736,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1096920</xdr:colOff>
+      <xdr:colOff>1096560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1748,8 +1751,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1301400" y="10772280"/>
-          <a:ext cx="1832400" cy="2444760"/>
+          <a:off x="1302120" y="10772280"/>
+          <a:ext cx="1832040" cy="2444400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1775,9 +1778,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92880</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1786,8 +1789,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358440" y="10725120"/>
-          <a:ext cx="6648480" cy="2257920"/>
+          <a:off x="3358800" y="10725120"/>
+          <a:ext cx="6649200" cy="2257560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2034,9 +2037,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1096920</xdr:colOff>
+      <xdr:colOff>1096560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2049,8 +2052,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1301400" y="10772280"/>
-          <a:ext cx="1832400" cy="2444760"/>
+          <a:off x="1302120" y="10772280"/>
+          <a:ext cx="1832040" cy="2444400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2080,7 +2083,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -2135,7 +2138,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 10</v>
+        <v>Version: 11</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -4109,7 +4112,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -4164,7 +4167,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 10</v>
+        <v>Version: 11</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -6138,7 +6141,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -6193,7 +6196,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 10</v>
+        <v>Version: 11</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -8157,13 +8160,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -8182,7 +8185,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="61"/>
     </row>
@@ -8276,6 +8279,14 @@
       </c>
       <c r="B15" s="0" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add end-state liveplot to dossier, update ga spreadsheet
* remember that "llist=list" makes a pointer, not a copy ... use copy()
* some attempt to audit core dumps, thanks Max
* put para/perp in GA spreadsheet
* pass command to consumer to save liveplot at end of scan
* add to html for dossier liveplot
* add retraction distance to GA spreadsheet
* up version number on all spreadsheets
</commit_message>
<xml_diff>
--- a/startup/xlsx/doublewheel.xlsx
+++ b/startup/xlsx/doublewheel.xlsx
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="74">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t xml:space="preserve">add a third motor to the grid spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added orientation and retraction distance to glancing angle spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -1176,9 +1179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1187,8 +1190,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358800" y="10725120"/>
-          <a:ext cx="6649200" cy="2257560"/>
+          <a:off x="3359520" y="10725120"/>
+          <a:ext cx="6649200" cy="2257200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1435,9 +1438,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1096920</xdr:colOff>
+      <xdr:colOff>1096560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1450,8 +1453,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1302480" y="10772280"/>
-          <a:ext cx="1832040" cy="2444400"/>
+          <a:off x="1303200" y="10772280"/>
+          <a:ext cx="1831680" cy="2444040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1477,9 +1480,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1488,8 +1491,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358800" y="10725120"/>
-          <a:ext cx="6649200" cy="2257560"/>
+          <a:off x="3359520" y="10725120"/>
+          <a:ext cx="6649200" cy="2257200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1736,9 +1739,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1096560</xdr:colOff>
+      <xdr:colOff>1096200</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1751,8 +1754,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1302120" y="10772280"/>
-          <a:ext cx="1832040" cy="2444400"/>
+          <a:off x="1302840" y="10772280"/>
+          <a:ext cx="1831680" cy="2444040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1778,9 +1781,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1789,8 +1792,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358800" y="10725120"/>
-          <a:ext cx="6649200" cy="2257560"/>
+          <a:off x="3359520" y="10725120"/>
+          <a:ext cx="6649200" cy="2257200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2037,9 +2040,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1096560</xdr:colOff>
+      <xdr:colOff>1096200</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2052,8 +2055,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1302120" y="10772280"/>
-          <a:ext cx="1832040" cy="2444400"/>
+          <a:off x="1302840" y="10772280"/>
+          <a:ext cx="1831680" cy="2444040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2083,7 +2086,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -2138,7 +2141,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 11</v>
+        <v>Version: 12</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -4112,7 +4115,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -4167,7 +4170,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 11</v>
+        <v>Version: 12</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -6141,7 +6144,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -6196,7 +6199,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 11</v>
+        <v>Version: 12</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -8160,13 +8163,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -8185,7 +8188,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="61"/>
     </row>
@@ -8287,6 +8290,14 @@
       </c>
       <c r="B16" s="0" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>